<commit_message>
create new branch 06_23_2023-09-29AM
</commit_message>
<xml_diff>
--- a/Planets/misc/revolutions per earth year.xlsx
+++ b/Planets/misc/revolutions per earth year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\VS Code\Abigail - vsCode\Planets\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4CA55AD-583A-4627-9E94-26A21F682576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65DA6C9-16A8-40EB-B0A0-A91FA5DA8517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3492DDAA-41AB-4962-A1EE-4DA5A6C31092}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3492DDAA-41AB-4962-A1EE-4DA5A6C31092}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,153 +411,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACDE92F-F334-4BC2-B18B-01AEAE2841E8}">
-  <dimension ref="C4:J8"/>
+  <dimension ref="B4:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.796875" style="1"/>
-    <col min="3" max="3" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.796875" style="1"/>
-    <col min="6" max="6" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.796875" style="1"/>
+    <col min="1" max="1" width="8.796875" style="1"/>
+    <col min="2" max="2" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.796875" style="1"/>
+    <col min="5" max="5" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="1" t="s">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C5" s="1">
+        <v>0.38700000000000001</v>
+      </c>
       <c r="D5" s="1">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="E5" s="1">
         <f>47.4 * 1000</f>
         <v>47400</v>
       </c>
+      <c r="E5" s="1">
+        <f>C5/D5</f>
+        <v>8.1645569620253162E-6</v>
+      </c>
       <c r="F5" s="1">
-        <f>D5/E5</f>
-        <v>8.1645569620253162E-6</v>
+        <f t="shared" ref="F5:F8" si="0">E5/$E$7</f>
+        <v>0.24316499999999996</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" ref="G5:G8" si="0">F5/$F$7</f>
-        <v>0.24316499999999996</v>
+        <f>1/F5</f>
+        <v>4.1124339440297746</v>
       </c>
       <c r="H5" s="1">
-        <f>1/G5</f>
-        <v>4.1124339440297746</v>
+        <v>88</v>
       </c>
       <c r="I5" s="1">
-        <v>88</v>
-      </c>
-      <c r="J5" s="1">
-        <f t="shared" ref="J5:J6" si="1">$I$7/I5</f>
+        <f t="shared" ref="I5:I6" si="1">$H$7/H5</f>
         <v>4.1477272727272725</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C6" s="1" t="s">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C6" s="1">
+        <v>0.72299999999999998</v>
+      </c>
       <c r="D6" s="1">
-        <v>0.72299999999999998</v>
-      </c>
-      <c r="E6" s="1">
         <f>35.02 * 1000</f>
         <v>35020</v>
       </c>
+      <c r="E6" s="1">
+        <f t="shared" ref="E6:E8" si="2">C6/D6</f>
+        <v>2.0645345516847514E-5</v>
+      </c>
       <c r="F6" s="1">
-        <f t="shared" ref="F6:F8" si="2">D6/E6</f>
-        <v>2.0645345516847514E-5</v>
-      </c>
-      <c r="G6" s="1">
         <f t="shared" si="0"/>
         <v>0.61488032552826943</v>
       </c>
+      <c r="G6" s="1">
+        <f t="shared" ref="G6:G8" si="3">1/F6</f>
+        <v>1.6263327325376009</v>
+      </c>
       <c r="H6" s="1">
-        <f t="shared" ref="H6:H8" si="3">1/G6</f>
-        <v>1.6263327325376009</v>
+        <v>225</v>
       </c>
       <c r="I6" s="1">
-        <v>225</v>
-      </c>
-      <c r="J6" s="1">
         <f t="shared" si="1"/>
         <v>1.6222222222222222</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="1" t="s">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
       <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
         <f>29.783 * 1000</f>
         <v>29783</v>
       </c>
+      <c r="E7" s="1">
+        <f>C7/D7</f>
+        <v>3.3576201188597525E-5</v>
+      </c>
       <c r="F7" s="1">
-        <f>D7/E7</f>
-        <v>3.3576201188597525E-5</v>
+        <f>E7/$E$7</f>
+        <v>1</v>
       </c>
       <c r="G7" s="1">
-        <f>F7/$F$7</f>
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
+      <c r="H7" s="1">
+        <v>365</v>
+      </c>
       <c r="I7" s="1">
-        <v>365</v>
-      </c>
-      <c r="J7" s="1">
-        <f>$I$7/I7</f>
+        <f>$H$7/H7</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="1" t="s">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C8" s="1">
+        <v>1.524</v>
+      </c>
       <c r="D8" s="1">
-        <v>1.524</v>
-      </c>
-      <c r="E8" s="1">
         <f>24.077 * 1000</f>
         <v>24077</v>
       </c>
-      <c r="F8" s="1">
+      <c r="E8" s="1">
         <f t="shared" si="2"/>
         <v>6.3296922374049926E-5</v>
       </c>
-      <c r="G8" s="1">
+      <c r="F8" s="1">
         <f t="shared" si="0"/>
         <v>1.8851722390663288</v>
       </c>
-      <c r="H8" s="1">
+      <c r="G8" s="1">
         <f t="shared" si="3"/>
         <v>0.53045550919807249</v>
       </c>
+      <c r="H8" s="1">
+        <v>687</v>
+      </c>
       <c r="I8" s="1">
-        <v>687</v>
-      </c>
-      <c r="J8" s="1">
-        <f>$I$7/I8</f>
+        <f>$H$7/H8</f>
         <v>0.53129548762736534</v>
       </c>
     </row>

</xml_diff>